<commit_message>
combining all of the football python scripts
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2024/Spreads/spreads_tracker_week17.xlsx
+++ b/PEAR/PEAR Football/y2024/Spreads/spreads_tracker_week17.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ESCAPE</t>
+          <t>PEAR</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -481,17 +481,17 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>ESCAPE ATS OPEN</t>
+          <t>PEAR ATS OPEN</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>ESCAPE ATS CLOSE</t>
+          <t>PEAR ATS CLOSE</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>ESCAPE SU</t>
+          <t>PEAR SU</t>
         </is>
       </c>
     </row>
@@ -766,41 +766,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8.199999999999999</v>
+        <v>8.600000000000001</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Penn State -nan</t>
+          <t>Ohio State -nan</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Penn State -9</t>
+          <t>Ohio State -7.5</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Penn State -17.2</t>
+          <t>Ohio State -16.1</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="I7" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Penn State -28</t>
+          <t>Ohio State -25</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -819,41 +819,41 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>7.9</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Washington -nan</t>
+          <t>Penn State -nan</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Washington -1</t>
+          <t>Penn State -9</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Louisville -6.9</t>
+          <t>Penn State -17.2</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I8" t="n">
-        <v>-1</v>
+        <v>28</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Louisville -1</t>
+          <t>Penn State -28</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -872,45 +872,45 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7.5</v>
+        <v>7.9</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>South Alabama -10.0</t>
+          <t>Washington -nan</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>South Alabama -6</t>
+          <t>Washington -1</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>South Alabama -13.5</t>
+          <t>Louisville -6.9</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>South Alabama -7</t>
+          <t>Louisville -1</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
         <v>1</v>
@@ -925,45 +925,45 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7.300000000000001</v>
+        <v>7.5</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Ohio State -nan</t>
+          <t>South Alabama -10.0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Ohio State -7.5</t>
+          <t>South Alabama -6</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Ohio State -14.8</t>
+          <t>South Alabama -13.5</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>7.5</v>
+        <v>-6</v>
       </c>
       <c r="I10" t="n">
-        <v>25</v>
+        <v>-7</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Ohio State -25</t>
+          <t>South Alabama -7</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -1243,41 +1243,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4.9</v>
+        <v>5.1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Memphis -2.0</t>
+          <t>Ohio State -2.5</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Memphis -5</t>
+          <t>Ohio State -2.5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Memphis -9.9</t>
+          <t>Ohio State -7.6</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>-5</v>
+        <v>-2.5</v>
       </c>
       <c r="I16" t="n">
-        <v>-5</v>
+        <v>-20</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Memphis -5</t>
+          <t>Ohio State -20</t>
         </is>
       </c>
       <c r="K16" t="n">
@@ -1296,41 +1296,41 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4.699999999999999</v>
+        <v>4.9</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Michigan -nan</t>
+          <t>Memphis -2.0</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Alabama -16.5</t>
+          <t>Memphis -5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Alabama -11.8</t>
+          <t>Memphis -9.9</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>-16.5</v>
+        <v>-5</v>
       </c>
       <c r="I17" t="n">
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Michigan -6</t>
+          <t>Memphis -5</t>
         </is>
       </c>
       <c r="K17" t="n">
@@ -1340,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1349,41 +1349,41 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4.5</v>
+        <v>4.699999999999999</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Vanderbilt -nan</t>
+          <t>Michigan -nan</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Georgia Tech -3</t>
+          <t>Alabama -16.5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Vanderbilt -1.5</t>
+          <t>Alabama -11.8</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>-3</v>
+        <v>-16.5</v>
       </c>
       <c r="I18" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Vanderbilt -8</t>
+          <t>Michigan -6</t>
         </is>
       </c>
       <c r="K18" t="n">
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="M18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1402,41 +1402,41 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Colorado State -nan</t>
+          <t>Vanderbilt -nan</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Miami (OH) -1</t>
+          <t>Georgia Tech -3</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Miami (OH) -5.4</t>
+          <t>Vanderbilt -1.5</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="I19" t="n">
-        <v>-26</v>
+        <v>8</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Miami (OH) -26</t>
+          <t>Vanderbilt -8</t>
         </is>
       </c>
       <c r="K19" t="n">
@@ -1455,48 +1455,48 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Notre Dame -nan</t>
+          <t>Colorado State -nan</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ohio State -8.5</t>
+          <t>Miami (OH) -1</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Ohio State -4.2</t>
+          <t>Miami (OH) -5.4</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>-8.5</v>
+        <v>-1</v>
       </c>
       <c r="I20" t="n">
-        <v>-11</v>
+        <v>-26</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Ohio State -11</t>
+          <t>Miami (OH) -26</t>
         </is>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
         <v>1</v>
@@ -1773,41 +1773,41 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Ohio State -2.5</t>
+          <t>San José State -2.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ohio State -2.5</t>
+          <t>South Florida -1.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Ohio State -6.3</t>
+          <t>South Florida -5.2</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>-2.5</v>
+        <v>-1.5</v>
       </c>
       <c r="I26" t="n">
-        <v>-20</v>
+        <v>-2</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Ohio State -20</t>
+          <t>South Florida -2</t>
         </is>
       </c>
       <c r="K26" t="n">
@@ -1826,41 +1826,41 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.7</v>
+        <v>3.300000000000001</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>San José State -2.5</t>
+          <t>Notre Dame -nan</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>South Florida -1.5</t>
+          <t>Notre Dame -7</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>South Florida -5.2</t>
+          <t>Notre Dame -10.3</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>-1.5</v>
+        <v>7</v>
       </c>
       <c r="I27" t="n">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>South Florida -2</t>
+          <t>Notre Dame -10</t>
         </is>
       </c>
       <c r="K27" t="n">
@@ -1875,7 +1875,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2091,48 +2091,48 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>UTSA -nan</t>
+          <t>Texas -nan</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>UTSA -12.5</t>
+          <t>Ohio State -6.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>UTSA -10.5</t>
+          <t>Ohio State -8.6</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>12.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I32" t="n">
-        <v>29</v>
+        <v>-14</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>UTSA -29</t>
+          <t>Ohio State -14</t>
         </is>
       </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" t="n">
         <v>1</v>
@@ -2144,48 +2144,48 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Arizona State -nan</t>
+          <t>UTSA -nan</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Texas -13.5</t>
+          <t>UTSA -12.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Texas -11.6</t>
+          <t>UTSA -10.5</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>-13.5</v>
+        <v>12.5</v>
       </c>
       <c r="I33" t="n">
-        <v>-8</v>
+        <v>29</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Texas -8</t>
+          <t>UTSA -29</t>
         </is>
       </c>
       <c r="K33" t="n">
         <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" t="n">
         <v>1</v>
@@ -2197,41 +2197,41 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.800000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Army -nan</t>
+          <t>Arizona State -nan</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Army -15</t>
+          <t>Texas -13.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Army -16.8</t>
+          <t>Texas -11.6</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>15</v>
+        <v>-13.5</v>
       </c>
       <c r="I34" t="n">
-        <v>21</v>
+        <v>-8</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Army -21</t>
+          <t>Texas -8</t>
         </is>
       </c>
       <c r="K34" t="n">
@@ -2250,41 +2250,41 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.3</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Nebraska -nan</t>
+          <t>Army -nan</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Nebraska -3</t>
+          <t>Army -15</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Nebraska -4.3</t>
+          <t>Army -16.8</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="I35" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Nebraska -5</t>
+          <t>Army -21</t>
         </is>
       </c>
       <c r="K35" t="n">
@@ -2303,12 +2303,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -2316,28 +2316,28 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>USC -nan</t>
+          <t>Nebraska -nan</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -3.5</t>
+          <t>Nebraska -3</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.2</t>
+          <t>Nebraska -4.3</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="I36" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>USC -4</t>
+          <t>Nebraska -5</t>
         </is>
       </c>
       <c r="K36" t="n">
@@ -2347,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -2356,41 +2356,41 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.199999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>TCU -nan</t>
+          <t>USC -nan</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>TCU -9.5</t>
+          <t>Texas A&amp;M -3.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>TCU -10.7</t>
+          <t>Texas A&amp;M -2.2</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>9.5</v>
+        <v>-3.5</v>
       </c>
       <c r="I37" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>TCU -31</t>
+          <t>USC -4</t>
         </is>
       </c>
       <c r="K37" t="n">
@@ -2400,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2409,51 +2409,51 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.1</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Bowling Green -6.5</t>
+          <t>TCU -nan</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Bowling Green -10.5</t>
+          <t>TCU -9.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Bowling Green -9.4</t>
+          <t>TCU -10.7</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="I38" t="n">
-        <v>-7</v>
+        <v>31</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Arkansas State -7</t>
+          <t>TCU -31</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" t="n">
         <v>1</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -2462,51 +2462,51 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.8999999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>UNLV -nan</t>
+          <t>Bowling Green -6.5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>UNLV -3</t>
+          <t>Bowling Green -10.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>UNLV -2.1</t>
+          <t>Bowling Green -9.4</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="I39" t="n">
-        <v>11</v>
+        <v>-7</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>UNLV -11</t>
+          <t>Arkansas State -7</t>
         </is>
       </c>
       <c r="K39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2515,48 +2515,48 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.7999999999999998</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Texas -nan</t>
+          <t>UNLV -nan</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Ohio State -6.5</t>
+          <t>UNLV -3</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Ohio State -7.3</t>
+          <t>UNLV -2.1</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>-6.5</v>
+        <v>3</v>
       </c>
       <c r="I40" t="n">
-        <v>-14</v>
+        <v>11</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Ohio State -14</t>
+          <t>UNLV -11</t>
         </is>
       </c>
       <c r="K40" t="n">
         <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
trying to improve football update efficiency
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2024/Spreads/spreads_tracker_week17.xlsx
+++ b/PEAR/PEAR Football/y2024/Spreads/spreads_tracker_week17.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>